<commit_message>
fix typo & add new test
</commit_message>
<xml_diff>
--- a/megaavr/extras/testCases/analogReadEnableDifferential/data.xlsx
+++ b/megaavr/extras/testCases/analogReadEnableDifferential/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sephi\Desktop\DxCore (cjeffries)\DxCore\megaavr\extras\testCases\analogReadEnableDifferential\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5007287-19F3-4FE8-ABB6-78330F8E1926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FF450A-CD78-4BF5-9BC2-534791CDAEB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-12885" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4685,7 +4685,7 @@
   <dimension ref="A1:O132"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A134" sqref="A134:XFD134"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>